<commit_message>
Rework PowerBI importer and add support for dedicated importKey column
</commit_message>
<xml_diff>
--- a/importer/budgeteer-powerbi-importer/src/test/resources/power-bi-example.xlsx
+++ b/importer/budgeteer-powerbi-importer/src/test/resources/power-bi-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czarnecki\Documents\adesso\budgeteer\importer\budgeteer-powerbi-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340D0429-1DDC-4742-9131-CD6FD456C6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E48DC3-DDA0-4891-8EDF-0232D3124AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-180" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>ProjektID</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Feste Mitarbeitende</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <dimension ref="A3:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,8 +541,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -570,8 +576,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>

</xml_diff>